<commit_message>
Sound volume added (gotta improve it later)
</commit_message>
<xml_diff>
--- a/7_LAWRENCE-ROUVEURE_SAWADOGO/TableauBord-LAWRENCE_SAWADOGO.xlsx
+++ b/7_LAWRENCE-ROUVEURE_SAWADOGO/TableauBord-LAWRENCE_SAWADOGO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\R1_01_InitiationDev_C#\SAE_1.01_1.02\7_LAWRENCE-ROUVEURE_SAWADOGO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hakim\Desktop\SAE\7_LAWRENCE-ROUVEURE_SAWADOGO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9259BD4-2F0F-4E9D-951C-A56894729BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB52867C-EC2F-4CF3-9C1E-07E3868001CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{926EDC97-D5E1-4CC0-AD68-C6D1DFEB1D8B}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="7845" xr2:uid="{926EDC97-D5E1-4CC0-AD68-C6D1DFEB1D8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de bord" sheetId="1" r:id="rId1"/>
@@ -29,15 +29,12 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Lundi 08/12</t>
   </si>
@@ -103,21 +100,8 @@
 Organisation + dépôt des livrables</t>
   </si>
   <si>
-    <t>2h Classe Ennemis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40min prise en main git
-maquette + répartition fonctionnalités
-Rédactions des règles /but
-</t>
-  </si>
-  <si>
     <t>40min prise en main git
 maquette + répartition fonctionnalités Rédactions des règles /but</t>
-  </si>
-  <si>
-    <t>Pathfinding
-Code de triche (Joueur &amp; Debug)</t>
   </si>
   <si>
     <t>Map aleatoire
@@ -125,17 +109,8 @@
 Generation Ennemis s/ map</t>
   </si>
   <si>
-    <t xml:space="preserve">Generation Ennemis s/map
-</t>
-  </si>
-  <si>
     <t>Classe Map
 Creation Map</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Selection Difficulté
-</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -152,6 +127,36 @@
 Collisions
 PickUp d'objet(armes &amp; potions)
 Code de triche (Joueur &amp; Debug)</t>
+  </si>
+  <si>
+    <t>40min prise en main git
+maquette + répartition fonctionnalités
+Rédactions des règles /but
+2h Classe Ennemis</t>
+  </si>
+  <si>
+    <t>2h fonctionnalitées
+de la classe ennemi</t>
+  </si>
+  <si>
+    <t>Pathfinding
+Code de triche (Joueur &amp; Debug)
+Côntroles d'utilisateur</t>
+  </si>
+  <si>
+    <t>Generation Ennemis s/map
+Collisions ennemis et
+joueur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Selection Difficulté
+Barre de vie
+</t>
+  </si>
+  <si>
+    <t>Menu son, parametres
+fix  etc..</t>
   </si>
 </sst>
 </file>
@@ -161,7 +166,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="[h]:mm:ss;@"/>
+    <numFmt numFmtId="165" formatCode="[h]:mm:ss;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -281,14 +286,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -324,36 +326,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="21" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -375,7 +374,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -673,11 +672,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E1F5600-0E64-4E20-9CCB-8407D1C0DC6A}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
@@ -705,121 +704,121 @@
       <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>0.16666666666666666</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>0.16666666666666699</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>0.16666666666666666</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="7">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="6">
         <f>SUM(C2:I2)</f>
         <v>0.75000000000000022</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="10"/>
+      <c r="G3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="19">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="19">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="19">
         <v>0.16666666666666666</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="19">
         <v>0.16666666666666666</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="19">
         <v>0.16666666666666666</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="23">
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="20">
         <f>SUM(C4:G4)</f>
         <v>0.74999999999999989</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="12"/>
+      <c r="G5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="11"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
@@ -832,95 +831,97 @@
       <c r="E8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>0.25</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>0.25</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <f>SUM(C9:E9)</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="21">
         <f>J2+F9</f>
         <v>1.3333333333333335</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="18" t="s">
+      <c r="C10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="23">
         <v>0.25</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="23">
         <v>0.25</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="20">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="24">
         <f>SUM(C11:E11)</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="21">
         <f>J4+F11</f>
         <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="19" t="s">
+      <c r="C12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G13" s="25">
+      <c r="G13" s="22">
         <f>G9+G11</f>
         <v>2.666666666666667</v>
       </c>

</xml_diff>